<commit_message>
First Version under the name IPS (Ice Protection System)
</commit_message>
<xml_diff>
--- a/Lunzer_Anti-Ice_Doc/Lunzer_Calk.xlsx
+++ b/Lunzer_Anti-Ice_Doc/Lunzer_Calk.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WA_Git\Arduino\Lunzer_Anti-Ice_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A39936-F774-4B71-9365-2E01906D3920}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61D5DBF-4475-431C-9248-05151CFB2503}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" xr2:uid="{CA07E164-EA75-4BEB-A9E5-E70DFFDEFC5D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" activeTab="1" xr2:uid="{CA07E164-EA75-4BEB-A9E5-E70DFFDEFC5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Strommessung" sheetId="1" r:id="rId1"/>
+    <sheet name="Spannungsmessung" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Referenz</t>
   </si>
@@ -75,6 +76,18 @@
   </si>
   <si>
     <t>Strom im Wandler</t>
+  </si>
+  <si>
+    <t>Eingangsspannung</t>
+  </si>
+  <si>
+    <t>Ausgangspannung</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
 </sst>
 </file>
@@ -110,8 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -428,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB4E485-7646-4CB6-8373-CFE02C62037E}">
   <dimension ref="B1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -557,4 +572,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4C38EC-9D25-4C27-A4E5-20A49DC9A5CD}">
+  <dimension ref="A3:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <f>47000+4700</f>
+        <v>51700</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <f>47000+4700</f>
+        <v>51700</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2">
+        <f>D3/(D5+D6)*D5</f>
+        <v>115.10204081632654</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <f>(F5*F5)/D5</f>
+        <v>0.25625686267085684</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <f>B5/(B3-B4)*B4</f>
+        <v>2247.826086956522</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>2200</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2">
+        <f>D3/(D5+D6)*D6</f>
+        <v>4.8979591836734695</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <f>(F6*F6)/D6</f>
+        <v>1.0904547347696036E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lunzer Test vor Ort
</commit_message>
<xml_diff>
--- a/Lunzer_Anti-Ice_Doc/Lunzer_Calk.xlsx
+++ b/Lunzer_Anti-Ice_Doc/Lunzer_Calk.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WA_Git\Arduino\Lunzer_Anti-Ice_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46DA365-82BE-440D-B05B-015966E23610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E49C06F-5922-4A72-BFA0-110DBA3E2F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" activeTab="1" xr2:uid="{CA07E164-EA75-4BEB-A9E5-E70DFFDEFC5D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" xr2:uid="{CA07E164-EA75-4BEB-A9E5-E70DFFDEFC5D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Strommessung" sheetId="1" r:id="rId1"/>
-    <sheet name="Spannungsmessung" sheetId="2" r:id="rId2"/>
+    <sheet name="Strommessung_Flieger" sheetId="3" r:id="rId1"/>
+    <sheet name="Strommessung_Test" sheetId="1" r:id="rId2"/>
+    <sheet name="Spannungsmessung" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>Referenz</t>
   </si>
@@ -440,11 +441,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3F1EAE-150B-4BE7-98ED-8C7E226CC223}">
+  <dimension ref="B1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1023</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <f>C6*$C$2</f>
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f>C6*$C$2/$C$1</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <f>C8*$C$3</f>
+        <v>0.23500000000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <f>C9*$C$4/$C$5</f>
+        <v>48.081000000000003</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>C10/C7</f>
+        <v>4.8081000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB4E485-7646-4CB6-8373-CFE02C62037E}">
   <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,11 +710,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4C38EC-9D25-4C27-A4E5-20A49DC9A5CD}">
   <dimension ref="A3:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>